<commit_message>
ajout du blaster pour les bombes
</commit_message>
<xml_diff>
--- a/Simul Collisions.xlsx
+++ b/Simul Collisions.xlsx
@@ -347,10 +347,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -372,15 +372,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>4764</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>4763</xdr:rowOff>
+      <xdr:colOff>9527</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>4763</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>4762</xdr:rowOff>
+      <xdr:colOff>9526</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -403,8 +403,272 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1052514" y="576263"/>
+          <a:off x="1057277" y="1438275"/>
           <a:ext cx="380999" cy="380999"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>23813</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>80963</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Image 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1071563" y="1824037"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>14288</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>71438</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Image 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1062038" y="2195512"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>14288</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>71438</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Image 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1443038" y="1466850"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>61913</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Image 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1814513" y="1462087"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Image 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="295275" y="1462087"/>
+          <a:ext cx="342900" cy="342900"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Image 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="666750" y="1457324"/>
+          <a:ext cx="342900" cy="342900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -706,7 +970,7 @@
   <dimension ref="A1:AG25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1"/>
+      <selection activeCell="AI16" sqref="AI16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,57 +980,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="38">
+      <c r="B1" s="39">
         <v>0</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38">
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39">
         <v>1</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38">
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39">
         <v>2</v>
       </c>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38">
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39">
         <v>3</v>
       </c>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38">
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39">
         <v>4</v>
       </c>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38">
+      <c r="S1" s="39"/>
+      <c r="T1" s="39"/>
+      <c r="U1" s="39"/>
+      <c r="V1" s="39">
         <v>5</v>
       </c>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38">
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39">
         <v>6</v>
       </c>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="38"/>
-      <c r="AC1" s="38"/>
-      <c r="AD1" s="38">
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39">
         <v>7</v>
       </c>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
     </row>
     <row r="2" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39">
+      <c r="A2" s="38">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
@@ -803,7 +1067,7 @@
       <c r="AG2" s="3"/>
     </row>
     <row r="3" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
+      <c r="A3" s="38"/>
       <c r="B3" s="4"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -838,7 +1102,7 @@
       <c r="AG3" s="6"/>
     </row>
     <row r="4" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
+      <c r="A4" s="38"/>
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
@@ -873,7 +1137,7 @@
       <c r="AG4" s="6"/>
     </row>
     <row r="5" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
+      <c r="A5" s="38"/>
       <c r="B5" s="20"/>
       <c r="C5" s="16"/>
       <c r="D5" s="16"/>
@@ -908,7 +1172,7 @@
       <c r="AG5" s="21"/>
     </row>
     <row r="6" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39">
+      <c r="A6" s="38">
         <v>1</v>
       </c>
       <c r="B6" s="22"/>
@@ -945,7 +1209,7 @@
       <c r="AG6" s="23"/>
     </row>
     <row r="7" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="39"/>
+      <c r="A7" s="38"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -980,7 +1244,7 @@
       <c r="AG7" s="6"/>
     </row>
     <row r="8" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="39"/>
+      <c r="A8" s="38"/>
       <c r="B8" s="4"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1015,7 +1279,7 @@
       <c r="AG8" s="6"/>
     </row>
     <row r="9" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="39"/>
+      <c r="A9" s="38"/>
       <c r="B9" s="20"/>
       <c r="C9" s="16"/>
       <c r="D9" s="16"/>
@@ -1050,7 +1314,7 @@
       <c r="AG9" s="21"/>
     </row>
     <row r="10" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="39">
+      <c r="A10" s="38">
         <v>2</v>
       </c>
       <c r="B10" s="22"/>
@@ -1087,7 +1351,7 @@
       <c r="AG10" s="23"/>
     </row>
     <row r="11" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="39"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="4"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
@@ -1122,7 +1386,7 @@
       <c r="AG11" s="6"/>
     </row>
     <row r="12" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="39"/>
+      <c r="A12" s="38"/>
       <c r="B12" s="4"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
@@ -1157,7 +1421,7 @@
       <c r="AG12" s="6"/>
     </row>
     <row r="13" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="39"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="20"/>
       <c r="C13" s="16"/>
       <c r="D13" s="16"/>
@@ -1192,7 +1456,7 @@
       <c r="AG13" s="21"/>
     </row>
     <row r="14" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="39">
+      <c r="A14" s="38">
         <v>3</v>
       </c>
       <c r="B14" s="22"/>
@@ -1229,7 +1493,7 @@
       <c r="AG14" s="23"/>
     </row>
     <row r="15" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="39"/>
+      <c r="A15" s="38"/>
       <c r="B15" s="4"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
@@ -1264,7 +1528,7 @@
       <c r="AG15" s="6"/>
     </row>
     <row r="16" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="39"/>
+      <c r="A16" s="38"/>
       <c r="B16" s="4"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -1299,7 +1563,7 @@
       <c r="AG16" s="6"/>
     </row>
     <row r="17" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="39"/>
+      <c r="A17" s="38"/>
       <c r="B17" s="20"/>
       <c r="C17" s="16"/>
       <c r="D17" s="16"/>
@@ -1334,7 +1598,7 @@
       <c r="AG17" s="21"/>
     </row>
     <row r="18" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="39">
+      <c r="A18" s="38">
         <v>4</v>
       </c>
       <c r="B18" s="22"/>
@@ -1371,7 +1635,7 @@
       <c r="AG18" s="23"/>
     </row>
     <row r="19" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="39"/>
+      <c r="A19" s="38"/>
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1406,7 +1670,7 @@
       <c r="AG19" s="6"/>
     </row>
     <row r="20" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="39"/>
+      <c r="A20" s="38"/>
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
@@ -1441,7 +1705,7 @@
       <c r="AG20" s="6"/>
     </row>
     <row r="21" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="39"/>
+      <c r="A21" s="38"/>
       <c r="B21" s="20"/>
       <c r="C21" s="16"/>
       <c r="D21" s="16"/>
@@ -1476,7 +1740,7 @@
       <c r="AG21" s="21"/>
     </row>
     <row r="22" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="39">
+      <c r="A22" s="38">
         <v>5</v>
       </c>
       <c r="B22" s="22"/>
@@ -1513,7 +1777,7 @@
       <c r="AG22" s="23"/>
     </row>
     <row r="23" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="39"/>
+      <c r="A23" s="38"/>
       <c r="B23" s="4"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
@@ -1548,7 +1812,7 @@
       <c r="AG23" s="6"/>
     </row>
     <row r="24" spans="1:33" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="39"/>
+      <c r="A24" s="38"/>
       <c r="B24" s="4"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1583,7 +1847,7 @@
       <c r="AG24" s="6"/>
     </row>
     <row r="25" spans="1:33" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="39"/>
+      <c r="A25" s="38"/>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>

</xml_diff>